<commit_message>
missed .xlsx file in commit
git-svn-id: file://localhost/tmp/svn2git/svn@2970 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/async-re/data/Refined_data_AL.xlsx
+++ b/papers/async-re/data/Refined_data_AL.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24600" windowHeight="15320" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24580" windowHeight="15320" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -102,11 +102,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="168" formatCode="0.000"/>
-    <numFmt numFmtId="170" formatCode="0.0"/>
-    <numFmt numFmtId="172" formatCode="0"/>
-  </numFmts>
   <fonts count="3">
     <font>
       <sz val="10"/>
@@ -145,7 +140,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -367,11 +362,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="522575432"/>
-        <c:axId val="522578920"/>
+        <c:axId val="528204552"/>
+        <c:axId val="527991544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="522575432"/>
+        <c:axId val="528204552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -387,14 +382,14 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="522578920"/>
+        <c:crossAx val="527991544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="522578920"/>
+        <c:axId val="527991544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -412,7 +407,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="522575432"/>
+        <c:crossAx val="528204552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -636,11 +631,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="522632344"/>
-        <c:axId val="522791976"/>
+        <c:axId val="454724616"/>
+        <c:axId val="454155720"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="522632344"/>
+        <c:axId val="454724616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -674,14 +669,14 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="522791976"/>
+        <c:crossAx val="454155720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="522791976"/>
+        <c:axId val="454155720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -699,7 +694,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="522632344"/>
+        <c:crossAx val="454724616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -806,10 +801,10 @@
           </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>'Andre Rework'!$B$2:$E$2</c:f>
+              <c:f>'Andre Rework'!$B$2:$F$2</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>4.0</c:v>
                 </c:pt>
@@ -821,16 +816,19 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Andre Rework'!$B$3:$E$3</c:f>
+              <c:f>'Andre Rework'!$B$3:$F$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>624.0</c:v>
                 </c:pt>
@@ -842,6 +840,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1023.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1432.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -863,10 +864,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'Andre Rework'!$B$2:$E$2</c:f>
+              <c:f>'Andre Rework'!$B$2:$F$2</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>4.0</c:v>
                 </c:pt>
@@ -878,16 +879,19 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Andre Rework'!$B$4:$E$4</c:f>
+              <c:f>'Andre Rework'!$B$4:$F$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>628.6</c:v>
                 </c:pt>
@@ -899,6 +903,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>804.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1014.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -920,10 +927,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'Andre Rework'!$B$2:$E$2</c:f>
+              <c:f>'Andre Rework'!$B$2:$F$2</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>4.0</c:v>
                 </c:pt>
@@ -935,16 +942,19 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Andre Rework'!$B$5:$E$5</c:f>
+              <c:f>'Andre Rework'!$B$5:$F$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>588.9</c:v>
                 </c:pt>
@@ -956,17 +966,20 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>641.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>650.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="473422360"/>
-        <c:axId val="473461208"/>
+        <c:axId val="457475352"/>
+        <c:axId val="457465912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="473422360"/>
+        <c:axId val="457475352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -978,10 +991,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1400"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE"/>
+                  <a:rPr lang="de-DE" sz="1400"/>
                   <a:t>Number of Replicas</a:t>
                 </a:r>
               </a:p>
@@ -991,14 +1004,24 @@
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="473461208"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1300"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="457465912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="473461208"/>
+        <c:axId val="457465912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1011,10 +1034,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1300"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE"/>
+                  <a:rPr lang="de-DE" sz="1300"/>
                   <a:t>Runtime (in sec)</a:t>
                 </a:r>
               </a:p>
@@ -1024,14 +1047,34 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="473422360"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1300"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="457475352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
       <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200"/>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -4984,16 +5027,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>939800</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>889000</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>914400</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5337,8 +5380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J3" sqref="J3:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -5619,10 +5662,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E5"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -5631,12 +5674,12 @@
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="B2" s="2">
         <v>4</v>
       </c>
@@ -5649,8 +5692,11 @@
       <c r="E2" s="2">
         <v>32</v>
       </c>
+      <c r="F2" s="2">
+        <v>64</v>
+      </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -5667,8 +5713,11 @@
       <c r="E3">
         <v>1023</v>
       </c>
+      <c r="F3">
+        <v>1432</v>
+      </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -5684,8 +5733,11 @@
       <c r="E4">
         <v>804</v>
       </c>
+      <c r="F4">
+        <v>1014</v>
+      </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -5701,13 +5753,16 @@
       <c r="E5">
         <v>641</v>
       </c>
+      <c r="F5">
+        <v>650</v>
+      </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:6">
       <c r="B9" t="s">
         <v>16</v>
       </c>
@@ -5721,7 +5776,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -5738,7 +5793,7 @@
         <v>18.34</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -5755,7 +5810,7 @@
         <v>13.4</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -5773,10 +5828,8 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="10" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">

</xml_diff>

<commit_message>
updates to the RE.ppt graphs
git-svn-id: file://localhost/tmp/svn2git/svn@3139 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/async-re/data/Refined_data_AL.xlsx
+++ b/papers/async-re/data/Refined_data_AL.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>Synchronous</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -66,6 +66,34 @@
   </si>
   <si>
     <t>16(4)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>4(16)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>8(32)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>16(64)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>32(128)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>64(256)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>128(512)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>256(1024)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -73,12 +101,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="3">
     <font>
       <sz val="10"/>
@@ -203,34 +225,33 @@
             </c:minus>
           </c:errBars>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:f>'Andre Rework'!$B$2:$H$2</c:f>
-              <c:numCache>
-                <c:formatCode>0</c:formatCode>
+              <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>4.0</c:v>
+                  <c:v>4(16)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.0</c:v>
+                  <c:v>8(32)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16.0</c:v>
+                  <c:v>16(64)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.0</c:v>
+                  <c:v>32(128)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>64.0</c:v>
+                  <c:v>64(256)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>128.0</c:v>
+                  <c:v>128(512)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>256.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>256(1024)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -325,34 +346,33 @@
             </c:minus>
           </c:errBars>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:f>'Andre Rework'!$B$2:$H$2</c:f>
-              <c:numCache>
-                <c:formatCode>0</c:formatCode>
+              <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>4.0</c:v>
+                  <c:v>4(16)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.0</c:v>
+                  <c:v>8(32)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16.0</c:v>
+                  <c:v>16(64)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.0</c:v>
+                  <c:v>32(128)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>64.0</c:v>
+                  <c:v>64(256)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>128.0</c:v>
+                  <c:v>128(512)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>256.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>256(1024)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -447,34 +467,33 @@
             </c:minus>
           </c:errBars>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:f>'Andre Rework'!$B$2:$H$2</c:f>
-              <c:numCache>
-                <c:formatCode>0</c:formatCode>
+              <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>4.0</c:v>
+                  <c:v>4(16)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.0</c:v>
+                  <c:v>8(32)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16.0</c:v>
+                  <c:v>16(64)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.0</c:v>
+                  <c:v>32(128)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>64.0</c:v>
+                  <c:v>64(256)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>128.0</c:v>
+                  <c:v>128(512)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>256.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>256(1024)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -508,11 +527,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="503970552"/>
-        <c:axId val="469591800"/>
+        <c:axId val="460957560"/>
+        <c:axId val="460965256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="503970552"/>
+        <c:axId val="460957560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -528,7 +547,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="de-DE" sz="1400"/>
-                  <a:t>Number of Replicas</a:t>
+                  <a:t>Number of Replicas(Number of Exchanges)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -547,14 +566,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="469591800"/>
+        <c:crossAx val="460965256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="469591800"/>
+        <c:axId val="460965256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -589,7 +608,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="503970552"/>
+        <c:crossAx val="460957560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -906,11 +925,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="495065752"/>
-        <c:axId val="503713672"/>
+        <c:axId val="460906568"/>
+        <c:axId val="460900040"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="495065752"/>
+        <c:axId val="460906568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -945,14 +964,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="503713672"/>
+        <c:crossAx val="460900040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="503713672"/>
+        <c:axId val="460900040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -987,7 +1006,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="495065752"/>
+        <c:crossAx val="460906568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1403,8 +1422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:H93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1419,26 +1438,26 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="B2" s="1">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1">
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="1">
-        <v>32</v>
-      </c>
-      <c r="F2" s="1">
-        <v>64</v>
-      </c>
-      <c r="G2" s="1">
-        <v>128</v>
-      </c>
-      <c r="H2" s="1">
-        <v>256</v>
+      <c r="G2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:8">

</xml_diff>

<commit_message>
updates to the abstract
git-svn-id: file://localhost/tmp/svn2git/svn@3229 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/async-re/data/Refined_data_AL.xlsx
+++ b/papers/async-re/data/Refined_data_AL.xlsx
@@ -673,11 +673,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="471342024"/>
-        <c:axId val="471489800"/>
+        <c:axId val="450936328"/>
+        <c:axId val="595962216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="471342024"/>
+        <c:axId val="450936328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -692,7 +692,7 @@
                   <a:defRPr lang="de-DE" sz="1400"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE" sz="1400"/>
+                  <a:rPr sz="1400"/>
                   <a:t>Number of Replicas(Number of Exchanges)</a:t>
                 </a:r>
               </a:p>
@@ -712,16 +712,17 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="471489800"/>
+        <c:crossAx val="595962216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="471489800"/>
+        <c:axId val="595962216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="500.0"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:title>
@@ -754,7 +755,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="471342024"/>
+        <c:crossAx val="450936328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1089,11 +1090,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="471558216"/>
-        <c:axId val="471564248"/>
+        <c:axId val="451252520"/>
+        <c:axId val="452246072"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="471558216"/>
+        <c:axId val="451252520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1109,7 +1110,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr sz="1400"/>
-                  <a:t>Number of Replicas</a:t>
+                  <a:t>Number of Replicas(Number of Exchanges)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1128,14 +1129,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="471564248"/>
+        <c:crossAx val="452246072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="471564248"/>
+        <c:axId val="452246072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="400.0"/>
@@ -1171,7 +1172,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="471558216"/>
+        <c:crossAx val="451252520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1506,11 +1507,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="471609384"/>
-        <c:axId val="471615416"/>
+        <c:axId val="468573848"/>
+        <c:axId val="452455608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="471609384"/>
+        <c:axId val="468573848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1526,7 +1527,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr sz="1400"/>
-                  <a:t>Number of Replicas</a:t>
+                  <a:t>Number of Replicas(Number of Exchanges)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1545,14 +1546,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="471615416"/>
+        <c:crossAx val="452455608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="471615416"/>
+        <c:axId val="452455608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="500.0"/>
@@ -1588,7 +1589,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="471609384"/>
+        <c:crossAx val="468573848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1923,11 +1924,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="471663176"/>
-        <c:axId val="471669208"/>
+        <c:axId val="468581640"/>
+        <c:axId val="450999496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="471663176"/>
+        <c:axId val="468581640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1943,7 +1944,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr sz="1400"/>
-                  <a:t>Number of Replicas</a:t>
+                  <a:t>Number of Replicas(Number of Exchanges)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1962,14 +1963,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="471669208"/>
+        <c:crossAx val="450999496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="471669208"/>
+        <c:axId val="450999496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2004,7 +2005,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="471663176"/>
+        <c:crossAx val="468581640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2339,11 +2340,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="471715304"/>
-        <c:axId val="471721336"/>
+        <c:axId val="451273176"/>
+        <c:axId val="463481912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="471715304"/>
+        <c:axId val="451273176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2359,7 +2360,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr sz="1400"/>
-                  <a:t>Number of Replicas</a:t>
+                  <a:t>Number of Replicas(Number of Exchanges)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2378,14 +2379,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="471721336"/>
+        <c:crossAx val="463481912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="471721336"/>
+        <c:axId val="463481912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="500.0"/>
@@ -2421,7 +2422,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="471715304"/>
+        <c:crossAx val="451273176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2655,7 +2656,7 @@
                   <c:v>600.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>660.0</c:v>
+                  <c:v>603.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>635.0</c:v>
@@ -2756,11 +2757,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="471768008"/>
-        <c:axId val="471774040"/>
+        <c:axId val="452086792"/>
+        <c:axId val="452092808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="471768008"/>
+        <c:axId val="452086792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2776,7 +2777,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr sz="1400"/>
-                  <a:t>Number of Replicas</a:t>
+                  <a:t>Number of Replicas(Number of Exchanges)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2795,14 +2796,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="471774040"/>
+        <c:crossAx val="452092808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="471774040"/>
+        <c:axId val="452092808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="500.0"/>
@@ -2838,7 +2839,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="471768008"/>
+        <c:crossAx val="452086792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3374,8 +3375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:H173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="L155" sqref="L155"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="L167" sqref="L167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -4580,7 +4581,7 @@
         <v>600</v>
       </c>
       <c r="C168">
-        <v>660</v>
+        <v>603</v>
       </c>
       <c r="D168">
         <v>635</v>
@@ -4645,6 +4646,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
graphs after more repeats of experiments
git-svn-id: file://localhost/tmp/svn2git/svn@3300 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/async-re/data/Refined_data_AL.xlsx
+++ b/papers/async-re/data/Refined_data_AL.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="43">
   <si>
     <t>Synchronous</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -188,11 +188,21 @@
     <t>32(128)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="3">
     <font>
       <sz val="10"/>
@@ -673,11 +683,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="471615944"/>
-        <c:axId val="468248776"/>
+        <c:axId val="464280200"/>
+        <c:axId val="451221704"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="471615944"/>
+        <c:axId val="464280200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -712,14 +722,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="468248776"/>
+        <c:crossAx val="451221704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="468248776"/>
+        <c:axId val="451221704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="500.0"/>
@@ -755,7 +765,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="471615944"/>
+        <c:crossAx val="464280200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1090,11 +1100,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="466168120"/>
-        <c:axId val="451128152"/>
+        <c:axId val="452637448"/>
+        <c:axId val="450898440"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="466168120"/>
+        <c:axId val="452637448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1129,14 +1139,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="451128152"/>
+        <c:crossAx val="450898440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="451128152"/>
+        <c:axId val="450898440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="400.0"/>
@@ -1172,7 +1182,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="466168120"/>
+        <c:crossAx val="452637448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1443,7 +1453,7 @@
                     <c:v>8.4</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>7.1</c:v>
+                    <c:v>4.57</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>2.0</c:v>
@@ -1461,7 +1471,7 @@
                     <c:v>8.4</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>7.1</c:v>
+                    <c:v>4.57</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>2.0</c:v>
@@ -1497,7 +1507,7 @@
                   <c:v>600.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>603.0</c:v>
+                  <c:v>606.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>635.0</c:v>
@@ -1507,11 +1517,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="467879896"/>
-        <c:axId val="452306568"/>
+        <c:axId val="595929112"/>
+        <c:axId val="463505816"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="467879896"/>
+        <c:axId val="595929112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1546,14 +1556,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="452306568"/>
+        <c:crossAx val="463505816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="452306568"/>
+        <c:axId val="463505816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="500.0"/>
@@ -1589,7 +1599,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="467879896"/>
+        <c:crossAx val="595929112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1860,7 +1870,7 @@
                     <c:v>27.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>4.6</c:v>
+                    <c:v>11.1</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>8.2</c:v>
@@ -1878,7 +1888,7 @@
                     <c:v>27.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>4.6</c:v>
+                    <c:v>11.1</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>8.2</c:v>
@@ -1914,7 +1924,7 @@
                   <c:v>568.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>641.0</c:v>
+                  <c:v>594.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>611.0</c:v>
@@ -1924,11 +1934,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="465946968"/>
-        <c:axId val="596115176"/>
+        <c:axId val="493513032"/>
+        <c:axId val="463944120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="465946968"/>
+        <c:axId val="493513032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1963,14 +1973,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="596115176"/>
+        <c:crossAx val="463944120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="596115176"/>
+        <c:axId val="463944120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2005,7 +2015,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="465946968"/>
+        <c:crossAx val="493513032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2273,10 +2283,10 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>9.0</c:v>
+                    <c:v>6.99</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>3.0</c:v>
+                    <c:v>10.79</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>4.0</c:v>
@@ -2291,10 +2301,10 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>9.0</c:v>
+                    <c:v>6.99</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>3.0</c:v>
+                    <c:v>10.79</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>4.0</c:v>
@@ -2327,10 +2337,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>607.0</c:v>
+                  <c:v>601.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>635.0</c:v>
+                  <c:v>621.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>626.0</c:v>
@@ -2340,11 +2350,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="452230344"/>
-        <c:axId val="466441496"/>
+        <c:axId val="586916952"/>
+        <c:axId val="468655736"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="452230344"/>
+        <c:axId val="586916952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2379,14 +2389,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="466441496"/>
+        <c:crossAx val="468655736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="466441496"/>
+        <c:axId val="468655736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="500.0"/>
@@ -2422,7 +2432,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="452230344"/>
+        <c:crossAx val="586916952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2602,7 +2612,7 @@
                     <c:v>8.4</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>7.1</c:v>
+                    <c:v>4.57</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>2.0</c:v>
@@ -2620,7 +2630,7 @@
                     <c:v>8.4</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>7.1</c:v>
+                    <c:v>4.57</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>2.0</c:v>
@@ -2656,7 +2666,7 @@
                   <c:v>600.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>660.0</c:v>
+                  <c:v>606.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>635.0</c:v>
@@ -2693,7 +2703,7 @@
                     <c:v>27.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>4.6</c:v>
+                    <c:v>11.1</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>8.2</c:v>
@@ -2711,7 +2721,7 @@
                     <c:v>27.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>4.6</c:v>
+                    <c:v>11.1</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>8.2</c:v>
@@ -2747,7 +2757,7 @@
                   <c:v>568.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>641.0</c:v>
+                  <c:v>594.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>611.0</c:v>
@@ -2757,11 +2767,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="464205768"/>
-        <c:axId val="494222520"/>
+        <c:axId val="471021592"/>
+        <c:axId val="464325048"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="464205768"/>
+        <c:axId val="471021592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2796,14 +2806,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="494222520"/>
+        <c:crossAx val="464325048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="494222520"/>
+        <c:axId val="464325048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="500.0"/>
@@ -2839,7 +2849,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="464205768"/>
+        <c:crossAx val="471021592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3375,8 +3385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:H173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
+      <selection activeCell="D125" sqref="D125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -3599,12 +3609,12 @@
         <v>25.4</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:5">
       <c r="B22" s="1" t="s">
         <v>10</v>
       </c>
@@ -3615,7 +3625,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -3632,7 +3642,7 @@
         <v>818.2</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -3646,7 +3656,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>2</v>
       </c>
@@ -3663,7 +3673,7 @@
         <v>636.20000000000005</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:5">
       <c r="B26" t="s">
         <v>29</v>
       </c>
@@ -3674,7 +3684,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:5">
       <c r="B27">
         <v>11.2</v>
       </c>
@@ -3685,7 +3695,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:5">
       <c r="B28">
         <v>0.35</v>
       </c>
@@ -3696,7 +3706,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:5">
       <c r="B29">
         <v>6</v>
       </c>
@@ -3707,12 +3717,17 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="30" spans="1:5">
+      <c r="E30" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:5">
       <c r="B32" s="1" t="s">
         <v>10</v>
       </c>
@@ -4284,7 +4299,7 @@
         <v>600</v>
       </c>
       <c r="C99">
-        <v>603</v>
+        <v>606</v>
       </c>
       <c r="D99">
         <v>635</v>
@@ -4328,7 +4343,7 @@
         <v>8.4</v>
       </c>
       <c r="C103">
-        <v>7.1</v>
+        <v>4.57</v>
       </c>
       <c r="D103">
         <v>2</v>
@@ -4391,7 +4406,7 @@
         <v>568</v>
       </c>
       <c r="C114">
-        <v>641</v>
+        <v>594</v>
       </c>
       <c r="D114">
         <v>611</v>
@@ -4435,7 +4450,7 @@
         <v>27</v>
       </c>
       <c r="C118">
-        <v>4.5999999999999996</v>
+        <v>11.1</v>
       </c>
       <c r="D118">
         <v>8.1999999999999993</v>
@@ -4490,10 +4505,10 @@
         <v>2</v>
       </c>
       <c r="B146">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="C146">
-        <v>635</v>
+        <v>621</v>
       </c>
       <c r="D146">
         <v>626</v>
@@ -4534,10 +4549,10 @@
     </row>
     <row r="150" spans="1:4">
       <c r="B150">
-        <v>9</v>
+        <v>6.99</v>
       </c>
       <c r="C150">
-        <v>3</v>
+        <v>10.79</v>
       </c>
       <c r="D150">
         <v>4</v>
@@ -4581,7 +4596,7 @@
         <v>600</v>
       </c>
       <c r="C168">
-        <v>660</v>
+        <v>606</v>
       </c>
       <c r="D168">
         <v>635</v>
@@ -4595,7 +4610,7 @@
         <v>568</v>
       </c>
       <c r="C169">
-        <v>641</v>
+        <v>594</v>
       </c>
       <c r="D169">
         <v>611</v>
@@ -4628,7 +4643,7 @@
         <v>8.4</v>
       </c>
       <c r="C172">
-        <v>7.1</v>
+        <v>4.57</v>
       </c>
       <c r="D172">
         <v>2</v>
@@ -4639,7 +4654,7 @@
         <v>27</v>
       </c>
       <c r="C173">
-        <v>4.5999999999999996</v>
+        <v>11.1</v>
       </c>
       <c r="D173">
         <v>8.1999999999999993</v>
@@ -4648,6 +4663,7 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">

</xml_diff>

<commit_message>
new figures for sync, cent and decent
git-svn-id: file://localhost/tmp/svn2git/svn@3304 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/async-re/data/Refined_data_AL.xlsx
+++ b/papers/async-re/data/Refined_data_AL.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="24800" windowHeight="16280" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28640" windowHeight="16240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Andre Rework" sheetId="2" r:id="rId1"/>
@@ -197,12 +197,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="3">
     <font>
       <sz val="10"/>
@@ -279,6 +273,21 @@
             <c:symbol val="diamond"/>
             <c:size val="7"/>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln>
+                <a:bevel/>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:errBars>
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
@@ -418,6 +427,16 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:errBars>
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
@@ -557,6 +576,16 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:errBars>
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
@@ -683,11 +712,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="464280200"/>
-        <c:axId val="451221704"/>
+        <c:axId val="69864968"/>
+        <c:axId val="69858568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="464280200"/>
+        <c:axId val="69864968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -722,14 +751,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="451221704"/>
+        <c:crossAx val="69858568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="451221704"/>
+        <c:axId val="69858568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="500.0"/>
@@ -765,7 +794,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="464280200"/>
+        <c:crossAx val="69864968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1100,11 +1129,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="452637448"/>
-        <c:axId val="450898440"/>
+        <c:axId val="514181240"/>
+        <c:axId val="514187256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="452637448"/>
+        <c:axId val="514181240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1139,14 +1168,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="450898440"/>
+        <c:crossAx val="514187256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="450898440"/>
+        <c:axId val="514187256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="400.0"/>
@@ -1182,7 +1211,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="452637448"/>
+        <c:crossAx val="514181240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1517,11 +1546,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="595929112"/>
-        <c:axId val="463505816"/>
+        <c:axId val="538779848"/>
+        <c:axId val="538793208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="595929112"/>
+        <c:axId val="538779848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1556,14 +1585,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="463505816"/>
+        <c:crossAx val="538793208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="463505816"/>
+        <c:axId val="538793208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="500.0"/>
@@ -1599,7 +1628,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="595929112"/>
+        <c:crossAx val="538779848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1934,11 +1963,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="493513032"/>
-        <c:axId val="463944120"/>
+        <c:axId val="548822472"/>
+        <c:axId val="548828488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="493513032"/>
+        <c:axId val="548822472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1973,14 +2002,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="463944120"/>
+        <c:crossAx val="548828488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="463944120"/>
+        <c:axId val="548828488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2015,7 +2044,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="493513032"/>
+        <c:crossAx val="548822472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2350,11 +2379,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="586916952"/>
-        <c:axId val="468655736"/>
+        <c:axId val="514407976"/>
+        <c:axId val="514413992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="586916952"/>
+        <c:axId val="514407976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2389,14 +2418,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="468655736"/>
+        <c:crossAx val="514413992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="468655736"/>
+        <c:axId val="514413992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="500.0"/>
@@ -2432,7 +2461,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="586916952"/>
+        <c:crossAx val="514407976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2767,11 +2796,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="471021592"/>
-        <c:axId val="464325048"/>
+        <c:axId val="514597432"/>
+        <c:axId val="514603448"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="471021592"/>
+        <c:axId val="514597432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2806,14 +2835,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="464325048"/>
+        <c:crossAx val="514603448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="464325048"/>
+        <c:axId val="514603448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="500.0"/>
@@ -2849,7 +2878,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="471021592"/>
+        <c:crossAx val="514597432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3385,8 +3414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:H173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
-      <selection activeCell="D125" sqref="D125"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V23" sqref="V23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -4663,7 +4692,6 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">

</xml_diff>

<commit_message>
equations and graphs: so much to do still
git-svn-id: file://localhost/tmp/svn2git/svn@3430 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/async-re/data/Refined_data_AL.xlsx
+++ b/papers/async-re/data/Refined_data_AL.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="44">
   <si>
     <t>Synchronous</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -180,6 +180,21 @@
     <t xml:space="preserve"> </t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>Synchronous</t>
+  </si>
+  <si>
+    <t>32(128)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>16(64)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>8(32)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -278,7 +293,18 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="2000"/>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:errBars>
@@ -426,7 +452,18 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="2000"/>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:errBars>
@@ -574,7 +611,18 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="2000"/>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:errBars>
@@ -703,11 +751,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="479066808"/>
-        <c:axId val="448312856"/>
+        <c:axId val="548865304"/>
+        <c:axId val="489861272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="479066808"/>
+        <c:axId val="548865304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -719,15 +767,16 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr lang="de-DE" sz="1400"/>
+                  <a:defRPr lang="de-DE" sz="2000"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="1400"/>
+                  <a:rPr sz="2000"/>
                   <a:t>Number of Replicas(Number of Exchanges)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
@@ -736,24 +785,25 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr lang="de-DE" sz="1300"/>
+              <a:defRPr lang="de-DE" sz="2000"/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="448312856"/>
+        <c:crossAx val="489861272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="448312856"/>
+        <c:axId val="489861272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="500.0"/>
         </c:scaling>
         <c:axPos val="l"/>
+        <c:majorGridlines/>
         <c:title>
           <c:tx>
             <c:rich>
@@ -761,15 +811,16 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr lang="de-DE" sz="1300"/>
+                  <a:defRPr lang="de-DE" sz="2000"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE" sz="1300"/>
+                  <a:rPr lang="de-DE" sz="2000"/>
                   <a:t>Runtime (in sec)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
@@ -778,24 +829,25 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr lang="de-DE" sz="1300"/>
+              <a:defRPr lang="de-DE" sz="2000"/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="479066808"/>
+        <c:crossAx val="548865304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr lang="de-DE" sz="1200"/>
+            <a:defRPr lang="de-DE" sz="2000"/>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
         </a:p>
@@ -1117,11 +1169,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="474000568"/>
-        <c:axId val="478665256"/>
+        <c:axId val="527549384"/>
+        <c:axId val="490278744"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="474000568"/>
+        <c:axId val="527549384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1156,14 +1208,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="478665256"/>
+        <c:crossAx val="490278744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="478665256"/>
+        <c:axId val="490278744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="400.0"/>
@@ -1199,7 +1251,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="474000568"/>
+        <c:crossAx val="527549384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1534,11 +1586,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="446245192"/>
-        <c:axId val="478846968"/>
+        <c:axId val="549495064"/>
+        <c:axId val="448153832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="446245192"/>
+        <c:axId val="549495064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1573,14 +1625,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="478846968"/>
+        <c:crossAx val="448153832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="478846968"/>
+        <c:axId val="448153832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="500.0"/>
@@ -1616,7 +1668,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="446245192"/>
+        <c:crossAx val="549495064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1951,11 +2003,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="490010008"/>
-        <c:axId val="448083208"/>
+        <c:axId val="451302360"/>
+        <c:axId val="446703704"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="490010008"/>
+        <c:axId val="451302360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1990,14 +2042,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="448083208"/>
+        <c:crossAx val="446703704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="448083208"/>
+        <c:axId val="446703704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2032,7 +2084,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="490010008"/>
+        <c:crossAx val="451302360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2083,6 +2135,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -2366,11 +2419,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="489098936"/>
-        <c:axId val="479154280"/>
+        <c:axId val="484792520"/>
+        <c:axId val="485143528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="489098936"/>
+        <c:axId val="484792520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2391,6 +2444,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
@@ -2404,14 +2458,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="479154280"/>
+        <c:crossAx val="485143528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="479154280"/>
+        <c:axId val="485143528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="500.0"/>
@@ -2433,6 +2487,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
@@ -2446,13 +2501,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="489098936"/>
+        <c:crossAx val="484792520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -2496,6 +2552,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -2779,11 +2836,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="451242488"/>
-        <c:axId val="454179528"/>
+        <c:axId val="528229736"/>
+        <c:axId val="496534232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="451242488"/>
+        <c:axId val="528229736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2804,6 +2861,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
@@ -2817,14 +2875,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="454179528"/>
+        <c:crossAx val="496534232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="454179528"/>
+        <c:axId val="496534232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="500.0"/>
@@ -2846,6 +2904,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
@@ -2859,13 +2918,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="451242488"/>
+        <c:crossAx val="528229736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -2891,98 +2951,83 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:style val="2"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000"/>
+              <a:t>32 replicas/128 exchanges</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Andre Rework'!$B$85</c:f>
+              <c:f>'Andre Rework'!$B$195</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>8(32)</c:v>
+                  <c:v>Synchronous</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:errBars>
+            <c:errDir val="y"/>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
             <c:plus>
               <c:numRef>
-                <c:f>('Andre Rework'!$B$90:$B$92,'Andre Rework'!$B$101:$B$103,'Andre Rework'!$B$116:$B$118)</c:f>
+                <c:f>'Andre Rework'!$B$200:$B$202</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="9"/>
+                  <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>11.2</c:v>
+                    <c:v>34.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>3.13</c:v>
+                    <c:v>10.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>27.0</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>5.6</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>1.7</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>8.4</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>6.0</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>9.0</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>27.0</c:v>
+                    <c:v>8.2</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>('Andre Rework'!$B$90:$B$92,'Andre Rework'!$B$101:$B$103,'Andre Rework'!$B$116:$B$118)</c:f>
+                <c:f>'Andre Rework'!$B$200:$B$202</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="9"/>
+                  <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>11.2</c:v>
+                    <c:v>34.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>3.13</c:v>
+                    <c:v>10.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>27.0</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>5.6</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>1.7</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>8.4</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>6.0</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>9.0</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>27.0</c:v>
+                    <c:v>8.2</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2990,9 +3035,9 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>('Andre Rework'!$A$86:$A$88,'Andre Rework'!$A$97:$A$99,'Andre Rework'!$A$112:$A$114)</c:f>
+              <c:f>'Andre Rework'!$A$196:$A$198</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>1M/4BJ</c:v>
                 </c:pt>
@@ -3000,24 +3045,6 @@
                   <c:v>2M/4BJ</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4M/4BJ</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1M/4BJ</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2M/4BJ</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4M/4BJ</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1M/4BJ</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2M/4BJ</c:v>
-                </c:pt>
-                <c:pt idx="8">
                   <c:v>4M/4BJ</c:v>
                 </c:pt>
               </c:strCache>
@@ -3025,36 +3052,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('Andre Rework'!$B$86:$B$88,'Andre Rework'!$B$97:$B$99,'Andre Rework'!$B$112:$B$114)</c:f>
+              <c:f>'Andre Rework'!$B$196:$B$198</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>608.0</c:v>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>715.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>625.0</c:v>
+                  <c:v>762.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>633.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>575.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>567.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>600.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>607.2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>606.4</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>568.0</c:v>
+                  <c:v>879.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3065,86 +3074,54 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Andre Rework'!$C$85</c:f>
+              <c:f>'Andre Rework'!$C$195</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>16(64)</c:v>
+                  <c:v>Asynchronous - Centralized</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:errBars>
+            <c:errDir val="y"/>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
             <c:plus>
               <c:numRef>
-                <c:f>('Andre Rework'!$C$90:$C$92,'Andre Rework'!$C$101:$C$103,'Andre Rework'!$C$116:$C$118)</c:f>
+                <c:f>'Andre Rework'!$C$200:$C$202</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="9"/>
+                  <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>17.0</c:v>
+                    <c:v>14.8</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>24.0</c:v>
+                    <c:v>2.4</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>4.6</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>16.9</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>3.4</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>4.57</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>23.0</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>3.0</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>11.1</c:v>
+                    <c:v>2.0</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>('Andre Rework'!$C$90:$C$92,'Andre Rework'!$C$101:$C$103,'Andre Rework'!$C$116:$C$118)</c:f>
+                <c:f>'Andre Rework'!$C$200:$C$202</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="9"/>
+                  <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>17.0</c:v>
+                    <c:v>14.8</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>24.0</c:v>
+                    <c:v>2.4</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>4.6</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>16.9</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>3.4</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>4.57</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>23.0</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>3.0</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>11.1</c:v>
+                    <c:v>2.0</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3152,9 +3129,9 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>('Andre Rework'!$A$86:$A$88,'Andre Rework'!$A$97:$A$99,'Andre Rework'!$A$112:$A$114)</c:f>
+              <c:f>'Andre Rework'!$A$196:$A$198</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>1M/4BJ</c:v>
                 </c:pt>
@@ -3162,24 +3139,6 @@
                   <c:v>2M/4BJ</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4M/4BJ</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1M/4BJ</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2M/4BJ</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4M/4BJ</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1M/4BJ</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2M/4BJ</c:v>
-                </c:pt>
-                <c:pt idx="8">
                   <c:v>4M/4BJ</c:v>
                 </c:pt>
               </c:strCache>
@@ -3187,36 +3146,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('Andre Rework'!$C$86:$C$88,'Andre Rework'!$C$97:$C$99,'Andre Rework'!$C$112:$C$114)</c:f>
+              <c:f>'Andre Rework'!$C$196:$C$198</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>648.0</c:v>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>633.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>702.0</c:v>
+                  <c:v>637.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>718.6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>560.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>591.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>606.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>618.4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>633.8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>594.0</c:v>
+                  <c:v>635.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3227,49 +3168,35 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Andre Rework'!$D$85</c:f>
+              <c:f>'Andre Rework'!$D$195</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>32(128)</c:v>
+                  <c:v>Asynchronous - Decentralized</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:errBars>
+            <c:errDir val="y"/>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
             <c:plus>
               <c:numRef>
-                <c:f>('Andre Rework'!$D$90:$D$92,'Andre Rework'!$D$101:$D$103,'Andre Rework'!$D$116:$D$118)</c:f>
+                <c:f>'Andre Rework'!$D$200:$D$202</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="9"/>
+                  <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>34.0</c:v>
+                    <c:v>2.4</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>10.0</c:v>
+                    <c:v>4.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>8.2</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>14.8</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>2.4</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>2.0</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>2.4</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>4.0</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
                     <c:v>8.2</c:v>
                   </c:pt>
                 </c:numCache>
@@ -3277,35 +3204,17 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>('Andre Rework'!$D$90:$D$92,'Andre Rework'!$D$101:$D$103,'Andre Rework'!$D$116:$D$118)</c:f>
+                <c:f>'Andre Rework'!$D$200:$D$202</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="9"/>
+                  <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>34.0</c:v>
+                    <c:v>2.4</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>10.0</c:v>
+                    <c:v>4.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>8.2</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>14.8</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>2.4</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>2.0</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>2.4</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>4.0</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
                     <c:v>8.2</c:v>
                   </c:pt>
                 </c:numCache>
@@ -3314,9 +3223,9 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>('Andre Rework'!$A$86:$A$88,'Andre Rework'!$A$97:$A$99,'Andre Rework'!$A$112:$A$114)</c:f>
+              <c:f>'Andre Rework'!$A$196:$A$198</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>1M/4BJ</c:v>
                 </c:pt>
@@ -3324,24 +3233,6 @@
                   <c:v>2M/4BJ</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4M/4BJ</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1M/4BJ</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2M/4BJ</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4M/4BJ</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1M/4BJ</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2M/4BJ</c:v>
-                </c:pt>
-                <c:pt idx="8">
                   <c:v>4M/4BJ</c:v>
                 </c:pt>
               </c:strCache>
@@ -3349,50 +3240,58 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('Andre Rework'!$D$86:$D$88,'Andre Rework'!$D$97:$D$99,'Andre Rework'!$D$112:$D$114)</c:f>
+              <c:f>'Andre Rework'!$D$196:$D$198</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>715.0</c:v>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>633.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>762.0</c:v>
+                  <c:v>623.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>879.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>633.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>637.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>635.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>633.8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>623.6</c:v>
-                </c:pt>
-                <c:pt idx="8">
                   <c:v>611.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="446057816"/>
-        <c:axId val="451741368"/>
-      </c:barChart>
+        <c:marker val="1"/>
+        <c:axId val="481937240"/>
+        <c:axId val="496543320"/>
+      </c:lineChart>
       <c:catAx>
-        <c:axId val="446057816"/>
+        <c:axId val="481937240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="496543320"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="496543320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="500.0"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
         <c:title>
           <c:tx>
             <c:rich>
@@ -3400,35 +3299,390 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2000"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1400"/>
-                  <a:t>Synchronous		Centralized		Decentralized</a:t>
+                  <a:rPr lang="en-US" sz="2000"/>
+                  <a:t>seconds</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="0.182588775667747"/>
-              <c:y val="0.928759894459103"/>
-            </c:manualLayout>
-          </c:layout>
+          <c:layout/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="451741368"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="481937240"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:style val="2"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000"/>
+              <a:t>16 replicas/64 exchanges</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Andre Rework'!$B$205</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Synchronous</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Andre Rework'!$B$210:$B$212</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>17.0</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>24.0</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>4.6</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Andre Rework'!$B$210:$B$212</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>17.0</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>24.0</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>4.6</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Andre Rework'!$A$206:$A$208</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1M/4BJ</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2M/4BJ</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4M/4BJ</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Andre Rework'!$B$206:$B$208</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>648.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>702.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>718.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Andre Rework'!$C$205</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Asynchronous - Centralized</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Andre Rework'!$C$210:$C$212</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>16.9</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>3.4</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>4.57</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Andre Rework'!$C$210:$C$212</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>16.9</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>3.4</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>4.57</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Andre Rework'!$A$206:$A$208</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1M/4BJ</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2M/4BJ</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4M/4BJ</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Andre Rework'!$C$206:$C$208</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>560.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>591.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>606.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Andre Rework'!$D$205</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Asynchronous - Decentralized</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Andre Rework'!$D$210:$D$212</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>23.0</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>3.0</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>11.1</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Andre Rework'!$D$210:$D$212</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>23.0</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>3.0</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>11.1</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Andre Rework'!$A$206:$A$208</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1M/4BJ</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2M/4BJ</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4M/4BJ</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Andre Rework'!$D$206:$D$208</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>618.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>633.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>594.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="484507608"/>
+        <c:axId val="447682392"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="484507608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="447682392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="451741368"/>
+        <c:axId val="447682392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="500.0"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
@@ -3443,7 +3697,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Seconds</a:t>
+                  <a:t>seconds</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -3452,7 +3706,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="446057816"/>
+        <c:crossAx val="484507608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3460,6 +3714,420 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="2000"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:style val="2"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000"/>
+              <a:t>8 replicas/32 exchanges</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Andre Rework'!$B$214</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Synchronous</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Andre Rework'!$B$219:$B$221</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>11.2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>3.13</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>27.0</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Andre Rework'!$B$219:$B$221</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>11.2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>3.13</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>27.0</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Andre Rework'!$A$215:$A$217</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1M/4BJ</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2M/4BJ</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4M/4BJ</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Andre Rework'!$B$215:$B$217</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>608.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>625.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>633.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Andre Rework'!$C$214</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Asynchronous - Centralized</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Andre Rework'!$C$219:$C$221</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>5.6</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.7</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>8.4</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Andre Rework'!$C$219:$C$221</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>5.6</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.7</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>8.4</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Andre Rework'!$A$215:$A$217</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1M/4BJ</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2M/4BJ</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4M/4BJ</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Andre Rework'!$C$215:$C$217</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>575.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>567.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>600.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Andre Rework'!$D$214</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Asynchronous - Decentralized</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Andre Rework'!$D$219:$D$221</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>6.0</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>9.0</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>27.0</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Andre Rework'!$D$219:$D$221</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>6.0</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>9.0</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>27.0</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Andre Rework'!$A$215:$A$217</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1M/4BJ</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2M/4BJ</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4M/4BJ</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Andre Rework'!$D$215:$D$217</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>607.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>606.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>568.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="527671864"/>
+        <c:axId val="528114216"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="527671864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="528114216"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="528114216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="500.0"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000"/>
+                  <a:t>seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="527671864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -3481,9 +4149,9 @@
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>850900</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3566,15 +4234,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>863600</xdr:colOff>
-      <xdr:row>114</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>137</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>135</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3655,20 +4323,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>812800</xdr:colOff>
-      <xdr:row>95</xdr:row>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>174</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>131</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>207</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="16" name="Chart 15"/>
+        <xdr:cNvPr id="27" name="Chart 26"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3678,6 +4346,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>216</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>251</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="29" name="Chart 28"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>216</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>251</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="30" name="Chart 29"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4006,10 +4734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:H173"/>
+  <dimension ref="A1:H221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J92" workbookViewId="0">
-      <selection activeCell="N110" sqref="N110"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -5283,6 +6011,311 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
+    <row r="195" spans="1:4">
+      <c r="A195" t="s">
+        <v>41</v>
+      </c>
+      <c r="B195" t="s">
+        <v>40</v>
+      </c>
+      <c r="C195" t="s">
+        <v>1</v>
+      </c>
+      <c r="D195" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4">
+      <c r="A196" t="s">
+        <v>30</v>
+      </c>
+      <c r="B196">
+        <v>715</v>
+      </c>
+      <c r="C196">
+        <v>633</v>
+      </c>
+      <c r="D196">
+        <f>641-0.3*24</f>
+        <v>633.79999999999995</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4">
+      <c r="A197" t="s">
+        <v>31</v>
+      </c>
+      <c r="B197">
+        <v>762</v>
+      </c>
+      <c r="C197">
+        <v>637</v>
+      </c>
+      <c r="D197">
+        <v>623.6</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4">
+      <c r="A198" t="s">
+        <v>32</v>
+      </c>
+      <c r="B198">
+        <v>879</v>
+      </c>
+      <c r="C198">
+        <v>635</v>
+      </c>
+      <c r="D198">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4">
+      <c r="B199" t="s">
+        <v>3</v>
+      </c>
+      <c r="C199" t="s">
+        <v>3</v>
+      </c>
+      <c r="D199" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4">
+      <c r="B200">
+        <v>34</v>
+      </c>
+      <c r="C200">
+        <v>14.8</v>
+      </c>
+      <c r="D200">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4">
+      <c r="B201">
+        <v>10</v>
+      </c>
+      <c r="C201">
+        <v>2.4</v>
+      </c>
+      <c r="D201">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4">
+      <c r="B202">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="C202">
+        <v>2</v>
+      </c>
+      <c r="D202">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4">
+      <c r="A205" t="s">
+        <v>42</v>
+      </c>
+      <c r="B205" t="s">
+        <v>40</v>
+      </c>
+      <c r="C205" t="s">
+        <v>1</v>
+      </c>
+      <c r="D205" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4">
+      <c r="A206" t="s">
+        <v>30</v>
+      </c>
+      <c r="B206">
+        <v>648</v>
+      </c>
+      <c r="C206">
+        <v>560</v>
+      </c>
+      <c r="D206">
+        <f>622-0.3*12</f>
+        <v>618.4</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4">
+      <c r="A207" t="s">
+        <v>31</v>
+      </c>
+      <c r="B207">
+        <v>702</v>
+      </c>
+      <c r="C207">
+        <v>591</v>
+      </c>
+      <c r="D207">
+        <f>635-0.3*4</f>
+        <v>633.79999999999995</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4">
+      <c r="A208" t="s">
+        <v>32</v>
+      </c>
+      <c r="B208">
+        <v>718.6</v>
+      </c>
+      <c r="C208">
+        <v>606</v>
+      </c>
+      <c r="D208">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4">
+      <c r="B209" t="s">
+        <v>3</v>
+      </c>
+      <c r="C209" t="s">
+        <v>3</v>
+      </c>
+      <c r="D209" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4">
+      <c r="B210">
+        <v>17</v>
+      </c>
+      <c r="C210">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="D210">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4">
+      <c r="B211">
+        <v>24</v>
+      </c>
+      <c r="C211">
+        <v>3.4</v>
+      </c>
+      <c r="D211">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4">
+      <c r="B212">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C212">
+        <v>4.57</v>
+      </c>
+      <c r="D212">
+        <v>11.1</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4">
+      <c r="A214" t="s">
+        <v>43</v>
+      </c>
+      <c r="B214" t="s">
+        <v>40</v>
+      </c>
+      <c r="C214" t="s">
+        <v>1</v>
+      </c>
+      <c r="D214" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4">
+      <c r="A215" t="s">
+        <v>30</v>
+      </c>
+      <c r="B215">
+        <v>608</v>
+      </c>
+      <c r="C215">
+        <v>575</v>
+      </c>
+      <c r="D215">
+        <f>609-0.3*6</f>
+        <v>607.20000000000005</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4">
+      <c r="A216" t="s">
+        <v>31</v>
+      </c>
+      <c r="B216">
+        <v>625</v>
+      </c>
+      <c r="C216">
+        <v>567</v>
+      </c>
+      <c r="D216">
+        <f>607-0.3*2</f>
+        <v>606.4</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4">
+      <c r="A217" t="s">
+        <v>32</v>
+      </c>
+      <c r="B217">
+        <v>633</v>
+      </c>
+      <c r="C217">
+        <v>600</v>
+      </c>
+      <c r="D217">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4">
+      <c r="B218" t="s">
+        <v>3</v>
+      </c>
+      <c r="C218" t="s">
+        <v>3</v>
+      </c>
+      <c r="D218" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4">
+      <c r="B219">
+        <v>11.2</v>
+      </c>
+      <c r="C219">
+        <v>5.6</v>
+      </c>
+      <c r="D219">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4">
+      <c r="B220">
+        <v>3.13</v>
+      </c>
+      <c r="C220">
+        <v>1.7</v>
+      </c>
+      <c r="D220">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4">
+      <c r="B221">
+        <v>27</v>
+      </c>
+      <c r="C221">
+        <v>8.4</v>
+      </c>
+      <c r="D221">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
resolving conflict. some work in section 5
git-svn-id: file://localhost/tmp/svn2git/svn@3523 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/async-re/data/Refined_data_AL.xlsx
+++ b/papers/async-re/data/Refined_data_AL.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28640" windowHeight="16240" tabRatio="500"/>
@@ -9,9 +9,9 @@
   <sheets>
     <sheet name="Andre Rework" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="130407" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -199,14 +199,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -250,7 +244,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -258,12 +252,22 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="1"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="101"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="1"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -311,6 +315,7 @@
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'Andre Rework'!$B$10:$H$10</c:f>
@@ -426,11 +431,12 @@
                   <c:v>1949.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2700.0</c:v>
+                  <c:v>3906.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -470,6 +476,7 @@
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'Andre Rework'!$B$11:$H$11</c:f>
@@ -585,11 +592,12 @@
                   <c:v>1393.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1800.0</c:v>
+                  <c:v>2411.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -629,6 +637,7 @@
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'Andre Rework'!$B$12:$H$12</c:f>
@@ -749,16 +758,27 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="548865304"/>
-        <c:axId val="489861272"/>
+        <c:smooth val="0"/>
+        <c:axId val="401017496"/>
+        <c:axId val="401022648"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="548865304"/>
+        <c:axId val="401017496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -770,15 +790,18 @@
                   <a:defRPr lang="de-DE" sz="2000"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="2000"/>
+                  <a:rPr lang="en-US" sz="2000"/>
                   <a:t>Number of Replicas(Number of Exchanges)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -790,18 +813,20 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="489861272"/>
+        <c:crossAx val="401022648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="489861272"/>
+        <c:axId val="401022648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="500.0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -821,8 +846,11 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -834,7 +862,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="548865304"/>
+        <c:crossAx val="401017496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -842,6 +870,7 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:layout/>
+      <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -854,6 +883,8 @@
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -867,7 +898,15 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="1"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="101"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="1"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -885,12 +924,14 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -913,6 +954,7 @@
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'Andre Rework'!$B$90:$D$90</c:f>
@@ -985,6 +1027,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1004,6 +1047,7 @@
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'Andre Rework'!$B$91:$D$91</c:f>
@@ -1076,6 +1120,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1095,6 +1140,7 @@
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'Andre Rework'!$B$92:$D$92</c:f>
@@ -1167,16 +1213,27 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="527549384"/>
-        <c:axId val="490278744"/>
+        <c:smooth val="0"/>
+        <c:axId val="401094120"/>
+        <c:axId val="401099736"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="527549384"/>
+        <c:axId val="401094120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -1194,9 +1251,11 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -1208,18 +1267,20 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="490278744"/>
+        <c:crossAx val="401099736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="490278744"/>
+        <c:axId val="401099736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="400.0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -1237,9 +1298,11 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -1251,14 +1314,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="527549384"/>
+        <c:crossAx val="401094120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
+      <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -1271,6 +1334,8 @@
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1284,7 +1349,15 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="1"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="101"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="1"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1302,12 +1375,14 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1330,6 +1405,7 @@
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'Andre Rework'!$B$101:$D$101</c:f>
@@ -1402,6 +1478,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1421,6 +1498,7 @@
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'Andre Rework'!$B$102:$D$102</c:f>
@@ -1493,6 +1571,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1512,6 +1591,7 @@
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'Andre Rework'!$B$103:$D$103</c:f>
@@ -1584,16 +1664,27 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="549495064"/>
-        <c:axId val="448153832"/>
+        <c:smooth val="0"/>
+        <c:axId val="401142216"/>
+        <c:axId val="401147864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="549495064"/>
+        <c:axId val="401142216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -1611,9 +1702,11 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -1625,18 +1718,20 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="448153832"/>
+        <c:crossAx val="401147864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="448153832"/>
+        <c:axId val="401147864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="500.0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -1654,9 +1749,11 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -1668,14 +1765,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="549495064"/>
+        <c:crossAx val="401142216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
+      <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -1688,6 +1785,8 @@
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1701,7 +1800,15 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="1"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="101"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="1"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1719,12 +1826,14 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1747,6 +1856,7 @@
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'Andre Rework'!$B$116:$D$116</c:f>
@@ -1819,6 +1929,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1838,6 +1949,7 @@
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'Andre Rework'!$B$117:$D$117</c:f>
@@ -1910,6 +2022,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1929,6 +2042,7 @@
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'Andre Rework'!$B$118:$D$118</c:f>
@@ -2001,16 +2115,27 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="451302360"/>
-        <c:axId val="446703704"/>
+        <c:smooth val="0"/>
+        <c:axId val="401191528"/>
+        <c:axId val="401197176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="451302360"/>
+        <c:axId val="401191528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -2028,9 +2153,11 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -2042,17 +2169,19 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="446703704"/>
+        <c:crossAx val="401197176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="446703704"/>
+        <c:axId val="401197176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -2070,9 +2199,11 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -2084,14 +2215,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="451302360"/>
+        <c:crossAx val="401191528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
+      <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -2104,6 +2235,8 @@
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -2117,7 +2250,15 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="1"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="101"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="1"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2135,12 +2276,14 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2163,6 +2306,7 @@
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'Andre Rework'!$B$148:$D$148</c:f>
@@ -2235,6 +2379,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2254,6 +2399,7 @@
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'Andre Rework'!$B$149:$D$149</c:f>
@@ -2326,6 +2472,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -2345,6 +2492,7 @@
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'Andre Rework'!$B$150:$D$150</c:f>
@@ -2417,16 +2565,27 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="484792520"/>
-        <c:axId val="485143528"/>
+        <c:smooth val="0"/>
+        <c:axId val="401240792"/>
+        <c:axId val="401246440"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="484792520"/>
+        <c:axId val="401240792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -2444,9 +2603,11 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -2458,18 +2619,20 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="485143528"/>
+        <c:crossAx val="401246440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="485143528"/>
+        <c:axId val="401246440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="500.0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -2487,9 +2650,11 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -2501,14 +2666,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="484792520"/>
+        <c:crossAx val="401240792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
+      <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -2521,6 +2686,8 @@
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -2534,7 +2701,15 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="1"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="101"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="1"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2552,12 +2727,14 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2580,6 +2757,7 @@
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'Andre Rework'!$B$171:$D$171</c:f>
@@ -2652,6 +2830,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2671,6 +2850,7 @@
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'Andre Rework'!$B$172:$D$172</c:f>
@@ -2743,6 +2923,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -2762,6 +2943,7 @@
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'Andre Rework'!$B$173:$D$173</c:f>
@@ -2834,16 +3016,27 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="528229736"/>
-        <c:axId val="496534232"/>
+        <c:smooth val="0"/>
+        <c:axId val="401290104"/>
+        <c:axId val="401295752"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="528229736"/>
+        <c:axId val="401290104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -2861,9 +3054,11 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -2875,18 +3070,20 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="496534232"/>
+        <c:crossAx val="401295752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="496534232"/>
+        <c:axId val="401295752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="500.0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -2904,9 +3101,11 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -2918,14 +3117,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="528229736"/>
+        <c:crossAx val="401290104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
+      <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -2938,6 +3137,8 @@
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -2951,7 +3152,15 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="2"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2969,12 +3178,14 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2996,6 +3207,7 @@
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'Andre Rework'!$B$200:$B$202</c:f>
@@ -3068,6 +3280,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -3090,6 +3303,7 @@
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'Andre Rework'!$C$200:$C$202</c:f>
@@ -3162,6 +3376,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -3184,6 +3399,7 @@
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'Andre Rework'!$D$200:$D$202</c:f>
@@ -3256,17 +3472,30 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="481937240"/>
-        <c:axId val="496543320"/>
+        <c:smooth val="0"/>
+        <c:axId val="401344888"/>
+        <c:axId val="401347976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="481937240"/>
+        <c:axId val="401344888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -3278,18 +3507,20 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="496543320"/>
+        <c:crossAx val="401347976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="496543320"/>
+        <c:axId val="401347976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="500.0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -3308,9 +3539,11 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -3322,14 +3555,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="481937240"/>
+        <c:crossAx val="401344888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -3342,6 +3575,8 @@
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -3355,7 +3590,15 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="2"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -3373,12 +3616,14 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -3400,6 +3645,7 @@
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'Andre Rework'!$B$210:$B$212</c:f>
@@ -3472,6 +3718,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -3494,6 +3741,7 @@
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'Andre Rework'!$C$210:$C$212</c:f>
@@ -3566,6 +3814,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -3588,6 +3837,7 @@
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'Andre Rework'!$D$210:$D$212</c:f>
@@ -3660,30 +3910,45 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="484507608"/>
-        <c:axId val="447682392"/>
+        <c:smooth val="0"/>
+        <c:axId val="401390776"/>
+        <c:axId val="401393832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="484507608"/>
+        <c:axId val="401390776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="447682392"/>
+        <c:crossAx val="401393832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="447682392"/>
+        <c:axId val="401393832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="500.0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -3702,20 +3967,24 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="484507608"/>
+        <c:crossAx val="401390776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:txPr>
     <a:bodyPr/>
@@ -3739,7 +4008,15 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="2"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -3757,12 +4034,14 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -3784,6 +4063,7 @@
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'Andre Rework'!$B$219:$B$221</c:f>
@@ -3856,6 +4136,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -3878,6 +4159,7 @@
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'Andre Rework'!$C$219:$C$221</c:f>
@@ -3950,6 +4232,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -3972,6 +4255,7 @@
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'Andre Rework'!$D$219:$D$221</c:f>
@@ -4044,17 +4328,30 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="527671864"/>
-        <c:axId val="528114216"/>
+        <c:smooth val="0"/>
+        <c:axId val="401437992"/>
+        <c:axId val="401441080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="527671864"/>
+        <c:axId val="401437992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -4066,18 +4363,20 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="528114216"/>
+        <c:crossAx val="401441080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="528114216"/>
+        <c:axId val="401441080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="500.0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -4096,9 +4395,11 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -4110,14 +4411,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="527671864"/>
+        <c:crossAx val="401437992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -4130,6 +4431,8 @@
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -4733,14 +5036,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
@@ -4799,7 +5102,7 @@
         <v>1949</v>
       </c>
       <c r="H3">
-        <v>2700</v>
+        <v>3906</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -4825,7 +5128,7 @@
         <v>1393</v>
       </c>
       <c r="H4">
-        <v>1800</v>
+        <v>2411</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -6321,7 +6624,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
added new data related to the large error bars and a note about the number of bigjob agents and machines
git-svn-id: file://localhost/tmp/svn2git/svn@3701 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/async-re/data/Refined_data_AL.xlsx
+++ b/papers/async-re/data/Refined_data_AL.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20515"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="17000" yWindow="100" windowWidth="10420" windowHeight="15120" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Andre Rework" sheetId="2" r:id="rId1"/>
@@ -314,7 +314,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:txPr>
                 <a:bodyPr/>
@@ -475,7 +474,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:txPr>
                 <a:bodyPr/>
@@ -636,7 +634,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:txPr>
                 <a:bodyPr/>
@@ -787,11 +784,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="523802136"/>
-        <c:axId val="523823288"/>
+        <c:axId val="390954328"/>
+        <c:axId val="390959480"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="523802136"/>
+        <c:axId val="390954328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -813,7 +810,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
@@ -830,7 +826,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="523823288"/>
+        <c:crossAx val="390959480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -838,7 +834,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="523823288"/>
+        <c:axId val="390959480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="500.0"/>
@@ -862,7 +858,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -879,14 +874,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="523802136"/>
+        <c:crossAx val="390954328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -1247,11 +1241,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="523728536"/>
-        <c:axId val="526492856"/>
+        <c:axId val="391032968"/>
+        <c:axId val="391036024"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="523728536"/>
+        <c:axId val="391032968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1260,7 +1254,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="526492856"/>
+        <c:crossAx val="391036024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1268,7 +1262,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="526492856"/>
+        <c:axId val="391036024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="500.0"/>
@@ -1280,7 +1274,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="523728536"/>
+        <c:crossAx val="391032968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1637,11 +1631,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="523751848"/>
-        <c:axId val="523754840"/>
+        <c:axId val="391075816"/>
+        <c:axId val="391078872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="523751848"/>
+        <c:axId val="391075816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1650,7 +1644,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="523754840"/>
+        <c:crossAx val="391078872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1658,7 +1652,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="523754840"/>
+        <c:axId val="391078872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="500.0"/>
@@ -1670,7 +1664,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="523751848"/>
+        <c:crossAx val="391075816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2027,11 +2021,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="523506648"/>
-        <c:axId val="523639848"/>
+        <c:axId val="411058776"/>
+        <c:axId val="411061832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="523506648"/>
+        <c:axId val="411058776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2040,7 +2034,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="523639848"/>
+        <c:crossAx val="411061832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2048,7 +2042,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="523639848"/>
+        <c:axId val="411061832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="500.0"/>
@@ -2060,7 +2054,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="523506648"/>
+        <c:crossAx val="411058776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2197,7 +2191,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1166.0</c:v>
+                  <c:v>949.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>900.0</c:v>
@@ -2400,11 +2394,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="526323336"/>
-        <c:axId val="526320536"/>
+        <c:axId val="411102312"/>
+        <c:axId val="411105368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="526323336"/>
+        <c:axId val="411102312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2413,7 +2407,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="526320536"/>
+        <c:crossAx val="411105368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2421,7 +2415,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="526320536"/>
+        <c:axId val="411105368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="500.0"/>
@@ -2433,7 +2427,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="526323336"/>
+        <c:crossAx val="411102312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2797,11 +2791,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="523605544"/>
-        <c:axId val="523588760"/>
+        <c:axId val="411146664"/>
+        <c:axId val="411149720"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="523605544"/>
+        <c:axId val="411146664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2810,7 +2804,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="523588760"/>
+        <c:crossAx val="411149720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2818,9 +2812,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="523588760"/>
+        <c:axId val="411149720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1000.0"/>
           <c:min val="500.0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -2830,7 +2825,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="523605544"/>
+        <c:crossAx val="411146664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3118,7 +3113,7 @@
                     <c:v>7.2</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>23.0</c:v>
+                    <c:v>3.5</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3136,7 +3131,7 @@
                     <c:v>7.2</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>23.0</c:v>
+                    <c:v>3.5</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3172,7 +3167,7 @@
                   <c:v>557.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>559.0</c:v>
+                  <c:v>570.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3189,11 +3184,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="523416856"/>
-        <c:axId val="523346904"/>
+        <c:axId val="411190424"/>
+        <c:axId val="411193480"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="523416856"/>
+        <c:axId val="411190424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3202,7 +3197,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="523346904"/>
+        <c:crossAx val="411193480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3210,9 +3205,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="523346904"/>
+        <c:axId val="411193480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1000.0"/>
           <c:min val="500.0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -3222,7 +3218,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="523416856"/>
+        <c:crossAx val="411190424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3787,7 +3783,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
       <selection activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
@@ -4035,7 +4031,7 @@
         <v>22</v>
       </c>
       <c r="B55">
-        <v>1166</v>
+        <v>949</v>
       </c>
       <c r="C55">
         <v>634</v>
@@ -4258,7 +4254,7 @@
         <v>600</v>
       </c>
       <c r="D77">
-        <v>559</v>
+        <v>570</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -4302,7 +4298,7 @@
         <v>9</v>
       </c>
       <c r="D81">
-        <v>23</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="115" spans="1:4">

</xml_diff>

<commit_message>
normalized data - scale-out
git-svn-id: file://localhost/tmp/svn2git/svn@3857 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/async-re/data/Refined_data_AL.xlsx
+++ b/papers/async-re/data/Refined_data_AL.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20515"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="21220" yWindow="0" windowWidth="28800" windowHeight="16460" tabRatio="500"/>
+    <workbookView xWindow="1220" yWindow="0" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Andre Rework" sheetId="2" r:id="rId1"/>
@@ -804,11 +804,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="482879544"/>
-        <c:axId val="385836056"/>
+        <c:axId val="444894344"/>
+        <c:axId val="529233800"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="482879544"/>
+        <c:axId val="444894344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -847,7 +847,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="385836056"/>
+        <c:crossAx val="529233800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -855,7 +855,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="385836056"/>
+        <c:axId val="529233800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="500.0"/>
@@ -896,7 +896,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="482879544"/>
+        <c:crossAx val="444894344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1265,11 +1265,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="405893912"/>
-        <c:axId val="464244600"/>
+        <c:axId val="434375176"/>
+        <c:axId val="427155608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="405893912"/>
+        <c:axId val="434375176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1278,7 +1278,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="464244600"/>
+        <c:crossAx val="427155608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1286,7 +1286,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="464244600"/>
+        <c:axId val="427155608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="500.0"/>
@@ -1298,7 +1298,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="405893912"/>
+        <c:crossAx val="434375176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1657,11 +1657,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="482999208"/>
-        <c:axId val="482896184"/>
+        <c:axId val="431825896"/>
+        <c:axId val="431828952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="482999208"/>
+        <c:axId val="431825896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1670,7 +1670,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="482896184"/>
+        <c:crossAx val="431828952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1678,7 +1678,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="482896184"/>
+        <c:axId val="431828952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="500.0"/>
@@ -1690,7 +1690,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="482999208"/>
+        <c:crossAx val="431825896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2049,11 +2049,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="467859048"/>
-        <c:axId val="482508216"/>
+        <c:axId val="426867576"/>
+        <c:axId val="426487320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="467859048"/>
+        <c:axId val="426867576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2062,7 +2062,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="482508216"/>
+        <c:crossAx val="426487320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2070,7 +2070,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="482508216"/>
+        <c:axId val="426487320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="500.0"/>
@@ -2082,7 +2082,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="467859048"/>
+        <c:crossAx val="426867576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2175,10 +2175,10 @@
                     <c:v>16.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>32.0</c:v>
+                    <c:v>18.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>18.0</c:v>
+                    <c:v>22.0</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2193,10 +2193,10 @@
                     <c:v>16.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>32.0</c:v>
+                    <c:v>18.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>18.0</c:v>
+                    <c:v>22.0</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2229,10 +2229,10 @@
                   <c:v>931.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>900.0</c:v>
+                  <c:v>988.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>879.0</c:v>
+                  <c:v>1017.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2328,7 +2328,7 @@
                   <c:v>656.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>635.0</c:v>
+                  <c:v>652.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2441,11 +2441,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="467008872"/>
-        <c:axId val="524803176"/>
+        <c:axId val="434490040"/>
+        <c:axId val="434493096"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="467008872"/>
+        <c:axId val="434490040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2454,7 +2454,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="524803176"/>
+        <c:crossAx val="434493096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2462,7 +2462,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="524803176"/>
+        <c:axId val="434493096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="500.0"/>
@@ -2474,7 +2474,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="467008872"/>
+        <c:crossAx val="434490040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2572,7 +2572,7 @@
                     <c:v>4.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>3.36</c:v>
+                    <c:v>8.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>5.0</c:v>
@@ -2590,7 +2590,7 @@
                     <c:v>4.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>3.36</c:v>
+                    <c:v>8.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>5.0</c:v>
@@ -2626,7 +2626,7 @@
                   <c:v>671.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>641.0</c:v>
+                  <c:v>691.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>721.0</c:v>
@@ -2838,11 +2838,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="467358824"/>
-        <c:axId val="524821352"/>
+        <c:axId val="434259208"/>
+        <c:axId val="434262264"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="467358824"/>
+        <c:axId val="434259208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2851,7 +2851,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="524821352"/>
+        <c:crossAx val="434262264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2859,7 +2859,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="524821352"/>
+        <c:axId val="434262264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000.0"/>
@@ -2872,7 +2872,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="467358824"/>
+        <c:crossAx val="434259208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3231,11 +3231,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="482515288"/>
-        <c:axId val="468121784"/>
+        <c:axId val="444721336"/>
+        <c:axId val="444724104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="482515288"/>
+        <c:axId val="444721336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3244,7 +3244,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="468121784"/>
+        <c:crossAx val="444724104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3252,7 +3252,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="468121784"/>
+        <c:axId val="444724104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000.0"/>
@@ -3265,7 +3265,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="482515288"/>
+        <c:crossAx val="444721336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3830,8 +3830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="D142" sqref="D142"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -4092,7 +4092,7 @@
         <v>23</v>
       </c>
       <c r="B56">
-        <v>900</v>
+        <v>988</v>
       </c>
       <c r="C56">
         <v>656</v>
@@ -4106,10 +4106,10 @@
         <v>15</v>
       </c>
       <c r="B57">
-        <v>879</v>
+        <v>1017.6</v>
       </c>
       <c r="C57">
-        <v>635</v>
+        <v>652</v>
       </c>
       <c r="D57" s="2">
         <v>608</v>
@@ -4139,7 +4139,7 @@
     </row>
     <row r="60" spans="1:4">
       <c r="B60">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="C60">
         <v>5</v>
@@ -4150,7 +4150,7 @@
     </row>
     <row r="61" spans="1:4">
       <c r="B61">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C61">
         <v>2</v>
@@ -4192,7 +4192,7 @@
         <v>23</v>
       </c>
       <c r="B66">
-        <v>641</v>
+        <v>691</v>
       </c>
       <c r="C66">
         <v>588</v>
@@ -4239,7 +4239,7 @@
     </row>
     <row r="70" spans="1:4">
       <c r="B70">
-        <v>3.36</v>
+        <v>8</v>
       </c>
       <c r="C70">
         <v>1.57</v>
@@ -4662,7 +4662,6 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
revisions, corrections, additions - sorry for the late commit
git-svn-id: file://localhost/tmp/svn2git/svn@4020 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/async-re/data/Refined_data_AL.xlsx
+++ b/papers/async-re/data/Refined_data_AL.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20515"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="0" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
+    <workbookView xWindow="-820" yWindow="140" windowWidth="15220" windowHeight="13900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Andre Rework" sheetId="2" r:id="rId1"/>
@@ -341,13 +341,13 @@
                     <c:v>17.0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>34.0</c:v>
+                    <c:v>19.0</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>52.0</c:v>
+                    <c:v>41.0</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.0</c:v>
+                    <c:v>50.0</c:v>
                   </c:pt>
                   <c:pt idx="6">
                     <c:v>50.0</c:v>
@@ -371,13 +371,13 @@
                     <c:v>17.0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>34.0</c:v>
+                    <c:v>19.0</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>52.0</c:v>
+                    <c:v>41.0</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.0</c:v>
+                    <c:v>50.0</c:v>
                   </c:pt>
                   <c:pt idx="6">
                     <c:v>50.0</c:v>
@@ -431,10 +431,10 @@
                   <c:v>802.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1023.0</c:v>
+                  <c:v>1008.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1389.0</c:v>
+                  <c:v>1403.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1949.0</c:v>
@@ -482,10 +482,10 @@
                     <c:v>16.36</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>13.4</c:v>
+                    <c:v>15.0</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>19.2</c:v>
+                    <c:v>23.0</c:v>
                   </c:pt>
                   <c:pt idx="5">
                     <c:v>50.0</c:v>
@@ -512,10 +512,10 @@
                     <c:v>16.36</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>13.4</c:v>
+                    <c:v>15.0</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>19.2</c:v>
+                    <c:v>23.0</c:v>
                   </c:pt>
                   <c:pt idx="5">
                     <c:v>50.0</c:v>
@@ -572,10 +572,10 @@
                   <c:v>701.83</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>804.0</c:v>
+                  <c:v>816.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1097.0</c:v>
+                  <c:v>1127.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1393.0</c:v>
@@ -623,10 +623,10 @@
                     <c:v>23.0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.4</c:v>
+                    <c:v>2.0</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.72</c:v>
+                    <c:v>2.0</c:v>
                   </c:pt>
                   <c:pt idx="5">
                     <c:v>8.5</c:v>
@@ -653,10 +653,10 @@
                     <c:v>23.0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.4</c:v>
+                    <c:v>2.0</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.72</c:v>
+                    <c:v>2.0</c:v>
                   </c:pt>
                   <c:pt idx="5">
                     <c:v>8.5</c:v>
@@ -713,10 +713,10 @@
                   <c:v>622.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>641.0</c:v>
+                  <c:v>642.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>659.0</c:v>
+                  <c:v>660.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>717.0</c:v>
@@ -739,11 +739,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="429115896"/>
-        <c:axId val="421413560"/>
+        <c:axId val="492085880"/>
+        <c:axId val="492091496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="429115896"/>
+        <c:axId val="492085880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -782,7 +782,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="421413560"/>
+        <c:crossAx val="492091496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -790,7 +790,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="421413560"/>
+        <c:axId val="492091496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -831,7 +831,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="429115896"/>
+        <c:crossAx val="492085880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1142,11 +1142,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="430501208"/>
-        <c:axId val="444897032"/>
+        <c:axId val="468455384"/>
+        <c:axId val="468409016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="430501208"/>
+        <c:axId val="468455384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1155,7 +1155,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="444897032"/>
+        <c:crossAx val="468409016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1163,7 +1163,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="444897032"/>
+        <c:axId val="468409016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -1175,7 +1175,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="430501208"/>
+        <c:crossAx val="468455384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1534,11 +1534,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="414303816"/>
-        <c:axId val="443822072"/>
+        <c:axId val="464658728"/>
+        <c:axId val="481256312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="414303816"/>
+        <c:axId val="464658728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1547,7 +1547,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="443822072"/>
+        <c:crossAx val="481256312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1555,7 +1555,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="443822072"/>
+        <c:axId val="481256312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="500.0"/>
@@ -1567,7 +1567,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="414303816"/>
+        <c:crossAx val="464658728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1619,7 +1619,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1926,11 +1925,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="430947496"/>
-        <c:axId val="450165352"/>
+        <c:axId val="428489832"/>
+        <c:axId val="467242536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="430947496"/>
+        <c:axId val="428489832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1939,7 +1938,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="450165352"/>
+        <c:crossAx val="467242536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1947,7 +1946,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="450165352"/>
+        <c:axId val="467242536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="500.0"/>
@@ -1959,14 +1958,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="430947496"/>
+        <c:crossAx val="428489832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2011,7 +2009,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2318,11 +2315,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="434917496"/>
-        <c:axId val="462345192"/>
+        <c:axId val="463696200"/>
+        <c:axId val="515619784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="434917496"/>
+        <c:axId val="463696200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2331,7 +2328,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="462345192"/>
+        <c:crossAx val="515619784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2339,7 +2336,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="462345192"/>
+        <c:axId val="515619784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="500.0"/>
@@ -2351,14 +2348,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="434917496"/>
+        <c:crossAx val="463696200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2710,11 +2706,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="414530296"/>
-        <c:axId val="445150536"/>
+        <c:axId val="468132120"/>
+        <c:axId val="425787464"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="414530296"/>
+        <c:axId val="468132120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2723,7 +2719,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="445150536"/>
+        <c:crossAx val="425787464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2731,7 +2727,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="445150536"/>
+        <c:axId val="425787464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -2743,7 +2739,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="414530296"/>
+        <c:crossAx val="468132120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3107,11 +3103,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="429108616"/>
-        <c:axId val="451824200"/>
+        <c:axId val="479089832"/>
+        <c:axId val="433613624"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="429108616"/>
+        <c:axId val="479089832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3120,7 +3116,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="451824200"/>
+        <c:crossAx val="433613624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3128,7 +3124,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="451824200"/>
+        <c:axId val="433613624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000.0"/>
@@ -3141,7 +3137,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="429108616"/>
+        <c:crossAx val="479089832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3500,11 +3496,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="430243960"/>
-        <c:axId val="463379064"/>
+        <c:axId val="492171448"/>
+        <c:axId val="468100584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="430243960"/>
+        <c:axId val="492171448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3513,7 +3509,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="463379064"/>
+        <c:crossAx val="468100584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3521,7 +3517,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="463379064"/>
+        <c:axId val="468100584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000.0"/>
@@ -3534,7 +3530,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="430243960"/>
+        <c:crossAx val="492171448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3835,11 +3831,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="443913016"/>
-        <c:axId val="444892360"/>
+        <c:axId val="421747416"/>
+        <c:axId val="491872760"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="443913016"/>
+        <c:axId val="421747416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3848,7 +3844,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="444892360"/>
+        <c:crossAx val="491872760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3856,7 +3852,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="444892360"/>
+        <c:axId val="491872760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -3868,7 +3864,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="443913016"/>
+        <c:crossAx val="421747416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4169,11 +4165,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="429169656"/>
-        <c:axId val="414383288"/>
+        <c:axId val="433585944"/>
+        <c:axId val="468328136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="429169656"/>
+        <c:axId val="433585944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4182,7 +4178,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="414383288"/>
+        <c:crossAx val="468328136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4190,7 +4186,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="414383288"/>
+        <c:axId val="468328136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -4202,7 +4198,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="429169656"/>
+        <c:crossAx val="433585944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4857,8 +4853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="A109" sqref="A109"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -4910,10 +4906,10 @@
         <v>802</v>
       </c>
       <c r="E3">
-        <v>1023</v>
+        <v>1008</v>
       </c>
       <c r="F3">
-        <v>1389</v>
+        <v>1403</v>
       </c>
       <c r="G3">
         <f>2845-896</f>
@@ -4937,10 +4933,10 @@
         <v>701.83</v>
       </c>
       <c r="E4">
-        <v>804</v>
+        <v>816</v>
       </c>
       <c r="F4">
-        <v>1097</v>
+        <v>1127</v>
       </c>
       <c r="G4">
         <v>1393</v>
@@ -4963,10 +4959,10 @@
         <v>622</v>
       </c>
       <c r="E5">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="F5">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="G5">
         <v>717</v>
@@ -5017,13 +5013,13 @@
         <v>17</v>
       </c>
       <c r="E10">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="F10">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="H10">
         <v>50</v>
@@ -5043,10 +5039,10 @@
         <v>16.36</v>
       </c>
       <c r="E11">
-        <v>13.4</v>
+        <v>15</v>
       </c>
       <c r="F11">
-        <v>19.2</v>
+        <v>23</v>
       </c>
       <c r="G11">
         <v>50</v>
@@ -5069,10 +5065,10 @@
         <v>23</v>
       </c>
       <c r="E12">
-        <v>2.4</v>
+        <v>2</v>
       </c>
       <c r="F12">
-        <v>0.72</v>
+        <v>2</v>
       </c>
       <c r="G12">
         <v>8.5</v>

</xml_diff>

<commit_message>
some pending commits -- crosswalks, etc.
git-svn-id: file://localhost/tmp/svn2git/svn@4510 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/async-re/data/Refined_data_AL.xlsx
+++ b/papers/async-re/data/Refined_data_AL.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20515"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20910"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-820" yWindow="140" windowWidth="15220" windowHeight="13900" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Andre Rework" sheetId="2" r:id="rId1"/>
@@ -320,6 +320,15 @@
             <c:symbol val="diamond"/>
             <c:size val="7"/>
           </c:marker>
+          <c:trendline>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:errBars>
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
@@ -461,6 +470,15 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:trendline>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:errBars>
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
@@ -602,6 +620,15 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:trendline>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:errBars>
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
@@ -739,11 +766,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="492085880"/>
-        <c:axId val="492091496"/>
+        <c:axId val="385785192"/>
+        <c:axId val="385792200"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="492085880"/>
+        <c:axId val="385785192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -782,7 +809,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="492091496"/>
+        <c:crossAx val="385792200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -790,7 +817,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="492091496"/>
+        <c:axId val="385792200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -831,7 +858,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="492085880"/>
+        <c:crossAx val="385785192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1142,11 +1169,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="468455384"/>
-        <c:axId val="468409016"/>
+        <c:axId val="406147992"/>
+        <c:axId val="406151048"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="468455384"/>
+        <c:axId val="406147992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1155,7 +1182,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="468409016"/>
+        <c:crossAx val="406151048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1163,7 +1190,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="468409016"/>
+        <c:axId val="406151048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -1175,7 +1202,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="468455384"/>
+        <c:crossAx val="406147992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1534,11 +1561,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="464658728"/>
-        <c:axId val="481256312"/>
+        <c:axId val="405807640"/>
+        <c:axId val="405810696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="464658728"/>
+        <c:axId val="405807640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1547,7 +1574,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="481256312"/>
+        <c:crossAx val="405810696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1555,7 +1582,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="481256312"/>
+        <c:axId val="405810696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="500.0"/>
@@ -1567,7 +1594,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="464658728"/>
+        <c:crossAx val="405807640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1619,6 +1646,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1925,11 +1953,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="428489832"/>
-        <c:axId val="467242536"/>
+        <c:axId val="405850712"/>
+        <c:axId val="405853768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="428489832"/>
+        <c:axId val="405850712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1938,7 +1966,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="467242536"/>
+        <c:crossAx val="405853768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1946,7 +1974,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="467242536"/>
+        <c:axId val="405853768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="500.0"/>
@@ -1958,13 +1986,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="428489832"/>
+        <c:crossAx val="405850712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2009,6 +2038,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2315,11 +2345,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="463696200"/>
-        <c:axId val="515619784"/>
+        <c:axId val="405894472"/>
+        <c:axId val="405897528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="463696200"/>
+        <c:axId val="405894472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2328,7 +2358,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="515619784"/>
+        <c:crossAx val="405897528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2336,7 +2366,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="515619784"/>
+        <c:axId val="405897528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="500.0"/>
@@ -2348,13 +2378,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="463696200"/>
+        <c:crossAx val="405894472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2706,11 +2737,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="468132120"/>
-        <c:axId val="425787464"/>
+        <c:axId val="405938088"/>
+        <c:axId val="405941144"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="468132120"/>
+        <c:axId val="405938088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2719,7 +2750,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="425787464"/>
+        <c:crossAx val="405941144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2727,7 +2758,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="425787464"/>
+        <c:axId val="405941144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -2739,7 +2770,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="468132120"/>
+        <c:crossAx val="405938088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3103,11 +3134,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="479089832"/>
-        <c:axId val="433613624"/>
+        <c:axId val="405982392"/>
+        <c:axId val="405985448"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="479089832"/>
+        <c:axId val="405982392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3116,7 +3147,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="433613624"/>
+        <c:crossAx val="405985448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3124,7 +3155,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="433613624"/>
+        <c:axId val="405985448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000.0"/>
@@ -3137,7 +3168,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="479089832"/>
+        <c:crossAx val="405982392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3496,11 +3527,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="492171448"/>
-        <c:axId val="468100584"/>
+        <c:axId val="406026184"/>
+        <c:axId val="406029240"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="492171448"/>
+        <c:axId val="406026184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3509,7 +3540,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="468100584"/>
+        <c:crossAx val="406029240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3517,7 +3548,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="468100584"/>
+        <c:axId val="406029240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000.0"/>
@@ -3530,7 +3561,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="492171448"/>
+        <c:crossAx val="406026184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3831,11 +3862,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="421747416"/>
-        <c:axId val="491872760"/>
+        <c:axId val="406066408"/>
+        <c:axId val="406069464"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="421747416"/>
+        <c:axId val="406066408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3844,7 +3875,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="491872760"/>
+        <c:crossAx val="406069464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3852,7 +3883,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="491872760"/>
+        <c:axId val="406069464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -3864,7 +3895,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="421747416"/>
+        <c:crossAx val="406066408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4165,11 +4196,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="433585944"/>
-        <c:axId val="468328136"/>
+        <c:axId val="406106680"/>
+        <c:axId val="406109736"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="433585944"/>
+        <c:axId val="406106680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4178,7 +4209,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="468328136"/>
+        <c:crossAx val="406109736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4186,7 +4217,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="468328136"/>
+        <c:axId val="406109736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -4198,7 +4229,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="433585944"/>
+        <c:crossAx val="406106680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4853,7 +4884,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H172"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>

</xml_diff>